<commit_message>
Add BigDecimal to XlsWriter.java
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticsWriter.xlsx
+++ b/src/main/resources/statisticsWriter.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Профиль обучения</t>
   </si>
@@ -29,6 +29,15 @@
     <t>Университеты</t>
   </si>
   <si>
+    <t>Математика</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Казанский Университет Вычислений;</t>
+  </si>
+  <si>
     <t>Лингвистика</t>
   </si>
   <si>
@@ -38,6 +47,9 @@
     <t>Медицина</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Московский Государственный Медицинский Университет;Тамбовский Университет Медицины;Самарский Медицинский Институт;</t>
   </si>
   <si>
@@ -45,12 +57,6 @@
   </si>
   <si>
     <t>Московский Выдуманный Университет;Московский Придуманный Институт;</t>
-  </si>
-  <si>
-    <t>Математика</t>
-  </si>
-  <si>
-    <t>Казанский Университет Вычислений;</t>
   </si>
 </sst>
 </file>
@@ -128,8 +134,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -138,58 +144,58 @@
         <v>1.0</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>4.329999923706055</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4.539999961853027</v>
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.0</v>
-      </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>